<commit_message>
Auto commit at 2025-10-16 14:57:28.62
</commit_message>
<xml_diff>
--- a/chargingdata/202509-202509.xlsx
+++ b/chargingdata/202509-202509.xlsx
@@ -820,39 +820,162 @@
     <xf numFmtId="179" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -862,148 +985,25 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1313,8 +1313,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1340,57 +1340,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51" t="s">
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="51"/>
+      <c r="M2" s="103"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="54"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="106"/>
     </row>
     <row r="4" spans="1:17" ht="27" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
@@ -1414,10 +1414,10 @@
       <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="55" t="s">
+      <c r="H4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="47"/>
+      <c r="I4" s="55"/>
       <c r="J4" s="3" t="s">
         <v>12</v>
       </c>
@@ -1432,7 +1432,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="100" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1453,10 +1453,10 @@
       <c r="G5" s="5">
         <v>6743.15</v>
       </c>
-      <c r="H5" s="46">
+      <c r="H5" s="53">
         <v>9535</v>
       </c>
-      <c r="I5" s="47"/>
+      <c r="I5" s="55"/>
       <c r="J5" s="2"/>
       <c r="K5" s="6">
         <v>2651.15</v>
@@ -1469,7 +1469,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A6" s="45"/>
+      <c r="A6" s="100"/>
       <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
@@ -1488,10 +1488,10 @@
       <c r="G6" s="5">
         <v>1912.37</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="53">
         <v>2885</v>
       </c>
-      <c r="I6" s="47"/>
+      <c r="I6" s="55"/>
       <c r="J6" s="2"/>
       <c r="K6" s="6">
         <v>772.35</v>
@@ -1504,7 +1504,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A7" s="45"/>
+      <c r="A7" s="100"/>
       <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1523,10 +1523,10 @@
       <c r="G7" s="10">
         <v>162.08000000000001</v>
       </c>
-      <c r="H7" s="48">
+      <c r="H7" s="101">
         <v>224</v>
       </c>
-      <c r="I7" s="49"/>
+      <c r="I7" s="85"/>
       <c r="J7" s="9"/>
       <c r="K7" s="6">
         <v>60.66</v>
@@ -1540,11 +1540,11 @@
       <c r="N7" s="11"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="58"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="99"/>
       <c r="D8" s="12">
         <v>302262.06</v>
       </c>
@@ -1557,7 +1557,7 @@
       <c r="G8" s="12">
         <v>8817.6</v>
       </c>
-      <c r="H8" s="59">
+      <c r="H8" s="88">
         <v>12644</v>
       </c>
       <c r="I8" s="60"/>
@@ -1575,10 +1575,10 @@
       <c r="O8" s="16"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="94" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1596,10 +1596,10 @@
       <c r="G9" s="5">
         <v>882.05</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="53">
         <v>1335</v>
       </c>
-      <c r="I9" s="47"/>
+      <c r="I9" s="55"/>
       <c r="J9" s="2">
         <v>205.63</v>
       </c>
@@ -1616,8 +1616,8 @@
       <c r="P9" s="16"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A10" s="62"/>
-      <c r="B10" s="63"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="94"/>
       <c r="C10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1633,10 +1633,10 @@
       <c r="G10" s="5">
         <v>2463.85</v>
       </c>
-      <c r="H10" s="46">
+      <c r="H10" s="53">
         <v>3862</v>
       </c>
-      <c r="I10" s="47"/>
+      <c r="I10" s="55"/>
       <c r="J10" s="2">
         <v>336.12</v>
       </c>
@@ -1654,10 +1654,10 @@
       <c r="Q10" s="16"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="65"/>
+      <c r="B11" s="80"/>
       <c r="C11" s="60"/>
       <c r="D11" s="12">
         <v>145618.5</v>
@@ -1671,7 +1671,7 @@
       <c r="G11" s="12">
         <v>3345.9</v>
       </c>
-      <c r="H11" s="59">
+      <c r="H11" s="88">
         <v>5197</v>
       </c>
       <c r="I11" s="60"/>
@@ -1691,11 +1691,11 @@
       <c r="O11" s="16"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="69"/>
-      <c r="C12" s="70"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="65"/>
       <c r="D12" s="17">
         <v>447880.56</v>
       </c>
@@ -1708,10 +1708,10 @@
       <c r="G12" s="17">
         <v>12163.5</v>
       </c>
-      <c r="H12" s="71">
+      <c r="H12" s="89">
         <v>17841</v>
       </c>
-      <c r="I12" s="70"/>
+      <c r="I12" s="65"/>
       <c r="J12" s="17">
         <v>541.75</v>
       </c>
@@ -1727,30 +1727,30 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="73"/>
-      <c r="L13" s="73"/>
-      <c r="M13" s="74"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="91"/>
+      <c r="L13" s="91"/>
+      <c r="M13" s="92"/>
     </row>
     <row r="14" spans="1:17" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="47"/>
+      <c r="C14" s="55"/>
       <c r="D14" s="3" t="s">
         <v>35</v>
       </c>
@@ -1763,10 +1763,10 @@
       <c r="G14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="55" t="s">
+      <c r="H14" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="47"/>
+      <c r="I14" s="55"/>
       <c r="J14" s="2" t="s">
         <v>40</v>
       </c>
@@ -1781,13 +1781,13 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A15" s="61" t="s">
+      <c r="A15" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="63"/>
+      <c r="C15" s="94"/>
       <c r="D15" s="2">
         <v>259380</v>
       </c>
@@ -1800,10 +1800,10 @@
       <c r="G15" s="5">
         <v>28891.119999999999</v>
       </c>
-      <c r="H15" s="76">
+      <c r="H15" s="95">
         <v>963.04</v>
       </c>
-      <c r="I15" s="77"/>
+      <c r="I15" s="96"/>
       <c r="J15" s="22">
         <v>0.1114</v>
       </c>
@@ -1818,11 +1818,11 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A16" s="62"/>
-      <c r="B16" s="75" t="s">
+      <c r="A16" s="83"/>
+      <c r="B16" s="93" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="63"/>
+      <c r="C16" s="94"/>
       <c r="D16" s="2">
         <v>75540</v>
       </c>
@@ -1835,10 +1835,10 @@
       <c r="G16" s="5">
         <v>8928.74</v>
       </c>
-      <c r="H16" s="76">
+      <c r="H16" s="95">
         <v>297.62</v>
       </c>
-      <c r="I16" s="77"/>
+      <c r="I16" s="96"/>
       <c r="J16" s="22">
         <v>0.1182</v>
       </c>
@@ -1854,10 +1854,10 @@
       <c r="O16" s="24"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="65"/>
+      <c r="B17" s="80"/>
       <c r="C17" s="60"/>
       <c r="D17" s="12">
         <v>334920</v>
@@ -1871,10 +1871,10 @@
       <c r="G17" s="12">
         <v>37819.86</v>
       </c>
-      <c r="H17" s="66">
+      <c r="H17" s="61">
         <v>1260.6600000000001</v>
       </c>
-      <c r="I17" s="67"/>
+      <c r="I17" s="62"/>
       <c r="J17" s="25">
         <f>(J15+J16)/2</f>
         <v>0.1148</v>
@@ -1896,7 +1896,7 @@
       <c r="A18" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="78" t="s">
+      <c r="B18" s="59" t="s">
         <v>49</v>
       </c>
       <c r="C18" s="60"/>
@@ -1912,10 +1912,10 @@
       <c r="G18" s="12">
         <v>14551.5</v>
       </c>
-      <c r="H18" s="66">
+      <c r="H18" s="61">
         <v>485.05</v>
       </c>
-      <c r="I18" s="67"/>
+      <c r="I18" s="62"/>
       <c r="J18" s="25">
         <v>9.0899999999999995E-2</v>
       </c>
@@ -1930,11 +1930,11 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="70"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="65"/>
       <c r="D19" s="17">
         <v>495090</v>
       </c>
@@ -1947,10 +1947,10 @@
       <c r="G19" s="17">
         <v>52371.360000000001</v>
       </c>
-      <c r="H19" s="79">
+      <c r="H19" s="66">
         <v>1745.71</v>
       </c>
-      <c r="I19" s="80"/>
+      <c r="I19" s="67"/>
       <c r="J19" s="27">
         <f>(J17+J18)/2</f>
         <v>0.10285</v>
@@ -1969,30 +1969,30 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="82"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="82"/>
-      <c r="E20" s="82"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82"/>
-      <c r="K20" s="82"/>
-      <c r="L20" s="82"/>
-      <c r="M20" s="83"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="50"/>
     </row>
     <row r="21" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="47"/>
+      <c r="C21" s="55"/>
       <c r="D21" s="3" t="s">
         <v>52</v>
       </c>
@@ -2005,10 +2005,10 @@
       <c r="G21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H21" s="55" t="s">
+      <c r="H21" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="I21" s="47"/>
+      <c r="I21" s="55"/>
       <c r="J21" s="3" t="s">
         <v>57</v>
       </c>
@@ -2023,13 +2023,13 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="82" t="s">
         <v>44</v>
       </c>
       <c r="B22" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="49"/>
+      <c r="C22" s="85"/>
       <c r="D22" s="28">
         <v>2.23</v>
       </c>
@@ -2042,10 +2042,10 @@
       <c r="G22" s="28">
         <v>26.25</v>
       </c>
-      <c r="H22" s="85">
+      <c r="H22" s="86">
         <v>34.18</v>
       </c>
-      <c r="I22" s="86"/>
+      <c r="I22" s="87"/>
       <c r="J22" s="28">
         <v>3.15</v>
       </c>
@@ -2060,11 +2060,11 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A23" s="62"/>
+      <c r="A23" s="83"/>
       <c r="B23" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="49"/>
+      <c r="C23" s="85"/>
       <c r="D23" s="28">
         <v>2.66</v>
       </c>
@@ -2077,10 +2077,10 @@
       <c r="G23" s="28">
         <v>33.58</v>
       </c>
-      <c r="H23" s="85">
+      <c r="H23" s="86">
         <v>34.83</v>
       </c>
-      <c r="I23" s="86"/>
+      <c r="I23" s="87"/>
       <c r="J23" s="28">
         <v>4.18</v>
       </c>
@@ -2095,10 +2095,10 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A24" s="64" t="s">
+      <c r="A24" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="65"/>
+      <c r="B24" s="80"/>
       <c r="C24" s="60"/>
       <c r="D24" s="14">
         <f>(D22+D23)/2</f>
@@ -2116,11 +2116,11 @@
         <f>(G22+G23)/2</f>
         <v>29.914999999999999</v>
       </c>
-      <c r="H24" s="66">
+      <c r="H24" s="61">
         <f>(H22+H23)/2</f>
         <v>34.504999999999995</v>
       </c>
-      <c r="I24" s="67"/>
+      <c r="I24" s="62"/>
       <c r="J24" s="14">
         <f>(J22+J23)/2</f>
         <v>3.665</v>
@@ -2142,7 +2142,7 @@
       <c r="A25" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="78" t="s">
+      <c r="B25" s="59" t="s">
         <v>49</v>
       </c>
       <c r="C25" s="60"/>
@@ -2158,10 +2158,10 @@
       <c r="G25" s="14">
         <v>33.99</v>
       </c>
-      <c r="H25" s="66">
+      <c r="H25" s="61">
         <v>43.52</v>
       </c>
-      <c r="I25" s="67"/>
+      <c r="I25" s="62"/>
       <c r="J25" s="14">
         <v>4.8099999999999996</v>
       </c>
@@ -2176,11 +2176,11 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A26" s="68" t="s">
+      <c r="A26" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="69"/>
-      <c r="C26" s="70"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="65"/>
       <c r="D26" s="18">
         <f>(D24+D25)/2</f>
         <v>2.7725</v>
@@ -2197,11 +2197,11 @@
         <f t="shared" si="4"/>
         <v>31.952500000000001</v>
       </c>
-      <c r="H26" s="79">
+      <c r="H26" s="66">
         <f>(H24+H25)/2</f>
         <v>39.012500000000003</v>
       </c>
-      <c r="I26" s="80"/>
+      <c r="I26" s="67"/>
       <c r="J26" s="18">
         <f>(J25+J24)/2</f>
         <v>4.2374999999999998</v>
@@ -2220,52 +2220,52 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A27" s="81" t="s">
+      <c r="A27" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="82"/>
-      <c r="C27" s="82"/>
-      <c r="D27" s="82"/>
-      <c r="E27" s="82"/>
-      <c r="F27" s="82"/>
-      <c r="G27" s="82"/>
-      <c r="H27" s="82"/>
-      <c r="I27" s="82"/>
-      <c r="J27" s="82"/>
-      <c r="K27" s="82"/>
-      <c r="L27" s="82"/>
-      <c r="M27" s="83"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="50"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A28" s="89" t="s">
+      <c r="A28" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="91" t="s">
+      <c r="B28" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="92"/>
-      <c r="D28" s="95" t="s">
+      <c r="C28" s="69"/>
+      <c r="D28" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="97" t="s">
+      <c r="E28" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="F28" s="98"/>
-      <c r="G28" s="98"/>
-      <c r="H28" s="98"/>
-      <c r="I28" s="98"/>
-      <c r="J28" s="99"/>
-      <c r="K28" s="97" t="s">
+      <c r="F28" s="75"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="75"/>
+      <c r="J28" s="76"/>
+      <c r="K28" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="L28" s="98"/>
-      <c r="M28" s="99"/>
+      <c r="L28" s="75"/>
+      <c r="M28" s="76"/>
     </row>
     <row r="29" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A29" s="90"/>
-      <c r="B29" s="93"/>
-      <c r="C29" s="94"/>
-      <c r="D29" s="96"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="73"/>
       <c r="E29" s="32" t="s">
         <v>69</v>
       </c>
@@ -2295,13 +2295,13 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A30" s="100" t="s">
+      <c r="A30" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="101" t="s">
+      <c r="B30" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="101"/>
+      <c r="C30" s="56"/>
       <c r="D30" s="5">
         <v>187961.01</v>
       </c>
@@ -2315,31 +2315,31 @@
         <v>1123.1500000000001</v>
       </c>
       <c r="H30" s="9">
-        <v>1028.97</v>
+        <v>509.14</v>
       </c>
       <c r="I30" s="35"/>
       <c r="J30" s="10">
         <f>IFERROR((I30+H30+G30+F30+E30),"")</f>
-        <v>128455.67</v>
+        <v>127935.84</v>
       </c>
       <c r="K30" s="2">
         <v>0.28999999999999998</v>
       </c>
       <c r="L30" s="36">
         <f>IFERROR((M30/D30),"")</f>
-        <v>0.31658342333870204</v>
+        <v>0.31934905010352949</v>
       </c>
       <c r="M30" s="37">
         <f>IFERROR((D30-J30),"")</f>
-        <v>59505.340000000011</v>
+        <v>60025.170000000013</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A31" s="100"/>
-      <c r="B31" s="101" t="s">
+      <c r="A31" s="77"/>
+      <c r="B31" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="101"/>
+      <c r="C31" s="56"/>
       <c r="D31" s="5">
         <v>54443.32</v>
       </c>
@@ -2353,31 +2353,31 @@
         <v>324.86</v>
       </c>
       <c r="H31" s="9">
-        <v>899.33</v>
+        <v>440.35</v>
       </c>
       <c r="I31" s="35"/>
       <c r="J31" s="10">
         <f>IFERROR((I31+H31+G31+F31+E31),"")</f>
-        <v>37753.950000000004</v>
+        <v>37294.97</v>
       </c>
       <c r="K31" s="2">
         <v>0.28999999999999998</v>
       </c>
       <c r="L31" s="36">
         <f t="shared" ref="L31:L35" si="6">IFERROR((M31/D31),"")</f>
-        <v>0.30654578008835603</v>
+        <v>0.31497619910027524</v>
       </c>
       <c r="M31" s="37">
         <f t="shared" ref="M31:M33" si="7">IFERROR((D31-J31),"")</f>
-        <v>16689.369999999995</v>
+        <v>17148.349999999999</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A32" s="100"/>
-      <c r="B32" s="102" t="s">
+      <c r="A32" s="77"/>
+      <c r="B32" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="101"/>
+      <c r="C32" s="56"/>
       <c r="D32" s="5">
         <v>3861.88</v>
       </c>
@@ -2391,30 +2391,30 @@
         <v>23.01</v>
       </c>
       <c r="H32" s="9">
-        <v>212.12</v>
+        <v>83.85</v>
       </c>
       <c r="I32" s="35"/>
       <c r="J32" s="10">
         <f>IFERROR((I32+H32+G32+F32+E32),"")</f>
-        <v>2349.4499999999998</v>
+        <v>2221.1799999999998</v>
       </c>
       <c r="K32" s="2">
         <v>0.28999999999999998</v>
       </c>
       <c r="L32" s="36">
         <f t="shared" si="6"/>
-        <v>0.39163050120666626</v>
+        <v>0.42484489419660898</v>
       </c>
       <c r="M32" s="37">
         <f>IFERROR((D32-J32),"")</f>
-        <v>1512.4300000000003</v>
+        <v>1640.7000000000003</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A33" s="64" t="s">
+      <c r="A33" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="65"/>
+      <c r="B33" s="80"/>
       <c r="C33" s="60"/>
       <c r="D33" s="12">
         <v>246266.21</v>
@@ -2430,34 +2430,34 @@
         <v>1471.0200000000002</v>
       </c>
       <c r="H33" s="13">
-        <f>H30+H31+H32</f>
-        <v>2140.42</v>
+        <f>SUM(H30:H32)</f>
+        <v>1033.3399999999999</v>
       </c>
       <c r="I33" s="13"/>
       <c r="J33" s="12">
         <f>IFERROR((I33+H33+G33+F33+E33),"")</f>
-        <v>168559.07</v>
+        <v>167451.99</v>
       </c>
       <c r="K33" s="15">
         <v>0.28000000000000003</v>
       </c>
       <c r="L33" s="38">
         <f t="shared" si="6"/>
-        <v>0.31554121858617951</v>
+        <v>0.32003667900683574</v>
       </c>
       <c r="M33" s="39">
         <f t="shared" si="7"/>
-        <v>77707.139999999985</v>
+        <v>78814.22</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A34" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="87" t="s">
+      <c r="B34" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="88"/>
+      <c r="C34" s="58"/>
       <c r="D34" s="12">
         <v>116024.98</v>
       </c>
@@ -2471,31 +2471,31 @@
         <v>696.15</v>
       </c>
       <c r="H34" s="13">
-        <v>973.02</v>
+        <v>607.63</v>
       </c>
       <c r="I34" s="13"/>
       <c r="J34" s="12">
         <f t="shared" ref="J34" si="8">IFERROR((I34+H34+G34+F34+E34),"")</f>
-        <v>88009.69</v>
+        <v>87644.3</v>
       </c>
       <c r="K34" s="15">
         <v>0.21</v>
       </c>
       <c r="L34" s="38">
         <f t="shared" si="6"/>
-        <v>0.24145912371628933</v>
+        <v>0.24460835933779082</v>
       </c>
       <c r="M34" s="39">
         <f>IFERROR((D34-J34),"")</f>
-        <v>28015.289999999994</v>
+        <v>28380.679999999993</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A35" s="105" t="s">
+      <c r="A35" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="105"/>
-      <c r="C35" s="105"/>
+      <c r="B35" s="47"/>
+      <c r="C35" s="47"/>
       <c r="D35" s="17">
         <v>362291.19</v>
       </c>
@@ -2511,67 +2511,67 @@
       </c>
       <c r="H35" s="19">
         <f>H34+H33</f>
-        <v>3113.44</v>
+        <v>1640.9699999999998</v>
       </c>
       <c r="I35" s="19"/>
       <c r="J35" s="17">
         <f>IFERROR((I35+H35+G35+F35+E35),"")</f>
-        <v>256568.75999999998</v>
+        <v>255096.28999999998</v>
       </c>
       <c r="K35" s="19">
         <v>0.26</v>
       </c>
       <c r="L35" s="40">
         <f t="shared" si="6"/>
-        <v>0.29181617692663192</v>
+        <v>0.29588050429821389</v>
       </c>
       <c r="M35" s="41">
         <f>IFERROR((D35-J35),"")</f>
-        <v>105722.43000000002</v>
+        <v>107194.90000000002</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A36" s="81" t="s">
+      <c r="A36" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="82"/>
-      <c r="C36" s="82"/>
-      <c r="D36" s="82"/>
-      <c r="E36" s="82"/>
-      <c r="F36" s="82"/>
-      <c r="G36" s="82"/>
-      <c r="H36" s="82"/>
-      <c r="I36" s="82"/>
-      <c r="J36" s="82"/>
-      <c r="K36" s="82"/>
-      <c r="L36" s="82"/>
-      <c r="M36" s="83"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="50"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A37" s="89" t="s">
+      <c r="A37" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="46" t="s">
+      <c r="B37" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="106"/>
-      <c r="D37" s="106"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="46" t="s">
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="G37" s="106"/>
-      <c r="H37" s="106"/>
-      <c r="I37" s="106"/>
-      <c r="J37" s="47"/>
-      <c r="K37" s="101" t="s">
+      <c r="G37" s="54"/>
+      <c r="H37" s="54"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="L37" s="101"/>
-      <c r="M37" s="101"/>
+      <c r="L37" s="56"/>
+      <c r="M37" s="56"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A38" s="90"/>
+      <c r="A38" s="52"/>
       <c r="B38" s="2" t="s">
         <v>83</v>
       </c>
@@ -2590,10 +2590,10 @@
       <c r="G38" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H38" s="101" t="s">
+      <c r="H38" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="I38" s="101"/>
+      <c r="I38" s="56"/>
       <c r="J38" s="2" t="s">
         <v>90</v>
       </c>
@@ -2629,11 +2629,11 @@
       <c r="G39" s="2">
         <v>12644</v>
       </c>
-      <c r="H39" s="103">
+      <c r="H39" s="45">
         <f>G39/F39</f>
         <v>0.74989621018919395</v>
       </c>
-      <c r="I39" s="104"/>
+      <c r="I39" s="46"/>
       <c r="J39" s="22">
         <v>0.72350000000000003</v>
       </c>
@@ -2669,11 +2669,11 @@
       <c r="G40" s="2">
         <v>5197</v>
       </c>
-      <c r="H40" s="103">
+      <c r="H40" s="45">
         <f>G40/F40</f>
         <v>0.9141600703605981</v>
       </c>
-      <c r="I40" s="104"/>
+      <c r="I40" s="46"/>
       <c r="J40" s="22">
         <v>0.75839999999999996</v>
       </c>
@@ -2690,15 +2690,49 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A36:M36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F37:J37"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A13:M13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A20:M20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="H23:I23"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="H25:I25"/>
@@ -2715,49 +2749,15 @@
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A20:M20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="A13:M13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A36:M36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F37:J37"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="H38:I38"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>